<commit_message>
Added new test - InvalidEmailApp().
</commit_message>
<xml_diff>
--- a/com.letsdeel/TestData/Data.xlsx
+++ b/com.letsdeel/TestData/Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t xml:space="preserve">Full Name</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">demo456user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mctestuser92.gmail.com</t>
   </si>
 </sst>
 </file>
@@ -398,7 +401,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -455,9 +458,18 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>

</xml_diff>